<commit_message>
add checkbos backend API test OK
</commit_message>
<xml_diff>
--- a/doc/設計書_FastAPIToDo.xlsx
+++ b/doc/設計書_FastAPIToDo.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\git\FastAPIToDo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B3A566-C644-4C6F-886D-160C5E5C4301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16246EF-5932-4362-83D2-BB7416776994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="画面" sheetId="1" r:id="rId1"/>
-    <sheet name="スキーマ" sheetId="2" r:id="rId2"/>
-    <sheet name="ソフト構造" sheetId="3" r:id="rId3"/>
+    <sheet name="ソフト構造" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,21 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>今のスキーマ</t>
-    <rPh sb="0" eb="1">
-      <t>イマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>追加スキーマ</t>
-    <rPh sb="0" eb="2">
-      <t>ツイカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>フロント</t>
     <phoneticPr fontId="1"/>
@@ -2693,6 +2678,153 @@
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" b="1"/>
             <a:t>イベントに関数登録。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>204109</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="テキスト ボックス 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A609C15B-3B06-6DD6-D669-FA6B985FF1D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3660322" y="3075215"/>
+          <a:ext cx="1442358" cy="639536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>チェックボックス</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>217713</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="テキスト ボックス 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A92F7704-E635-4642-831E-99D9FCEAF8E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7320642" y="3129643"/>
+          <a:ext cx="1442358" cy="639536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>チェックボックス</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>情報</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2980,37 +3112,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6645A3A3-F1C6-4266-98EF-4E0211009A7C}">
-  <dimension ref="B2:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
-  <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33D9D01-FCD6-466E-A65E-7EA43CAF5594}">
   <dimension ref="C1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75"/>
@@ -3020,10 +3126,10 @@
   <sheetData>
     <row r="1" spans="3:29">
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bag Fix: cannot save checkbox on editing
</commit_message>
<xml_diff>
--- a/doc/設計書_FastAPIToDo.xlsx
+++ b/doc/設計書_FastAPIToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\git\FastAPIToDo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16246EF-5932-4362-83D2-BB7416776994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC1F78-3CA1-48A6-B9DE-EB9293A156EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="画面" sheetId="1" r:id="rId1"/>
@@ -2717,7 +2717,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
+          <a:srgbClr val="FFC000"/>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -2787,7 +2787,84 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>チェックボックス</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>情報</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>217715</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>74</xdr:col>
+      <xdr:colOff>190502</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="テキスト ボックス 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A4E719-DD25-4806-9615-10BC9D922CE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16872858" y="2966357"/>
+          <a:ext cx="1442358" cy="639536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -3116,7 +3193,7 @@
   <dimension ref="C1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
tempolaly fix login page
</commit_message>
<xml_diff>
--- a/doc/設計書_FastAPIToDo.xlsx
+++ b/doc/設計書_FastAPIToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\git\FastAPIToDo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D96E98D-1904-4CF6-A12E-2C8B9C701FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24A193C-A048-427D-A8B8-27A8C1887206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,15 +516,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>142889</xdr:colOff>
+      <xdr:colOff>161926</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
+      <xdr:colOff>114303</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>166681</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -535,14 +535,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="7" idx="1"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="7048514" y="576262"/>
-          <a:ext cx="1295387" cy="66669"/>
+          <a:off x="7067551" y="566736"/>
+          <a:ext cx="1381127" cy="61914"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>

</xml_diff>